<commit_message>
changes related to auth physician field
</commit_message>
<xml_diff>
--- a/src/main/java/resources/RMSAllEnvTestData.xlsx
+++ b/src/main/java/resources/RMSAllEnvTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagababu.parepalli\eclipse-workspace\RmsCustomerPortal\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABFDA1A-5831-4D55-8D8C-7E38B745660E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACD72DE-F166-4AE7-ACF8-AC5F2B19C4FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1F45140C-9D0A-43A7-8AA8-1FFD7BE961DD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>NeedBydate</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Zarif.mohd</t>
   </si>
   <si>
-    <t>Kick4Thy</t>
-  </si>
-  <si>
     <t>Index</t>
   </si>
   <si>
@@ -120,6 +117,15 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Zarif@mohd</t>
+  </si>
+  <si>
+    <t>12/20/2021</t>
+  </si>
+  <si>
+    <t>12/21/2021</t>
   </si>
 </sst>
 </file>
@@ -492,7 +498,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,13 +525,14 @@
       <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
-        <v>24</v>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{4466BF9B-784B-4127-8094-26F3A482D028}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{D95AF64D-7218-4987-91D5-FF15423DFC06}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -536,14 +543,14 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -560,7 +567,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -586,7 +593,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -609,23 +616,23 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>26</v>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -639,14 +646,14 @@
       <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
+      <c r="H3" t="s">
+        <v>13</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>17</v>
+      <c r="J3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -660,7 +667,7 @@
   <dimension ref="F16:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:O17"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,7 +680,7 @@
         <v>4</v>
       </c>
       <c r="H16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I16" t="s">
         <v>6</v>
@@ -705,7 +712,7 @@
         <v>4</v>
       </c>
       <c r="H17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I17" t="s">
         <v>6</v>

</xml_diff>